<commit_message>
done changes in BasPage and TestData
</commit_message>
<xml_diff>
--- a/Excel/testdata.xlsx
+++ b/Excel/testdata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ADMIN\waytoautomation\AppiumPageObjectModel_1\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{897BB6C3-BA2C-4C11-A41E-8D7B116959CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6630A741-B4B5-45F7-8171-152CE744C891}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="990" yWindow="480" windowWidth="16815" windowHeight="14475" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,10 +35,10 @@
     <t>Hotel</t>
   </si>
   <si>
-    <t>Citymax Hotel Bur Dubai</t>
-  </si>
-  <si>
     <t>Airport Hotel Earth</t>
+  </si>
+  <si>
+    <t>Marco Polo Hotel</t>
   </si>
 </sst>
 </file>
@@ -423,7 +423,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -444,7 +444,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -452,7 +452,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
done changes in TestData
</commit_message>
<xml_diff>
--- a/Excel/testdata.xlsx
+++ b/Excel/testdata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ADMIN\waytoautomation\AppiumPageObjectModel_1\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6630A741-B4B5-45F7-8171-152CE744C891}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FF342FA-5EBD-4F06-BFCF-C0152F64A91F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="990" yWindow="480" windowWidth="16815" windowHeight="14475" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,10 +35,10 @@
     <t>Hotel</t>
   </si>
   <si>
-    <t>Airport Hotel Earth</t>
-  </si>
-  <si>
     <t>Marco Polo Hotel</t>
+  </si>
+  <si>
+    <t>Hotel the View</t>
   </si>
 </sst>
 </file>
@@ -423,7 +423,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -444,7 +444,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -452,7 +452,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>